<commit_message>
Actualizacion grafico de mediciones
Agrego 2 graficos nuevos con las mediciones que hizo Lucas.
</commit_message>
<xml_diff>
--- a/TP2B/GraficoDeMediciones.xlsx
+++ b/TP2B/GraficoDeMediciones.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Todos" sheetId="1" r:id="rId1"/>
+    <sheet name="Elementales" sheetId="2" r:id="rId2"/>
+    <sheet name="No Elementales" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Input</t>
   </si>
@@ -51,9 +51,6 @@
     <t>09_Vector100000ElementosAleatorio</t>
   </si>
   <si>
-    <t>11_Vector2097152ElementosAleatorio</t>
-  </si>
-  <si>
     <t>Seleccion</t>
   </si>
   <si>
@@ -76,6 +73,24 @@
   </si>
   <si>
     <t>Tiempo Algoritmo (ms)</t>
+  </si>
+  <si>
+    <t>Cantidad de elementos</t>
+  </si>
+  <si>
+    <t>Tiempo de ejecución del algoritmo (ms)</t>
+  </si>
+  <si>
+    <t>Selección</t>
+  </si>
+  <si>
+    <t>Inserción</t>
+  </si>
+  <si>
+    <t>QuickSort</t>
+  </si>
+  <si>
+    <t>Fusión</t>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -148,21 +163,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -185,7 +233,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Todos!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -196,7 +244,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Todos!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -235,7 +283,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:f>Todos!$C$3:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -279,7 +327,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Todos!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,7 +338,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Todos!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -329,7 +377,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:f>Todos!$D$3:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -373,7 +421,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Todos!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -384,7 +432,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Todos!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -423,7 +471,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:f>Todos!$E$3:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -462,23 +510,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="64603648"/>
-        <c:axId val="64602112"/>
+        <c:axId val="54650368"/>
+        <c:axId val="54651904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64603648"/>
+        <c:axId val="54650368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64602112"/>
+        <c:crossAx val="54651904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64602112"/>
+        <c:axId val="54651904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +534,742 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64603648"/>
+        <c:crossAx val="54650368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Todos!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Todos!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Todos!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Todos!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Quicksort</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Todos!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Todos!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Todos!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fusion</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Todos!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>350000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Todos!$H$3:$H$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="54771712"/>
+        <c:axId val="54773248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="54771712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54773248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="54773248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54771712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="es-AR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Elementales!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Burbujeo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Elementales!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Elementales!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>894</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3603</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14363</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18188</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21280</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30692</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>43989</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>57558</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73060</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>89752</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Elementales!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Inserción</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Elementales!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Elementales!$C$3:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1444</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5837</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7434</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9014</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12996</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17638</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23117</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29386</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36440</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Elementales!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Selección</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Elementales!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Elementales!$D$3:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>818</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1441</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4453</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5777</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7308</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9032</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12975</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17719</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23094</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>29346</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>36163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="101506432"/>
+        <c:axId val="101504896"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101506432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101504896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="101504896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101506432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -505,20 +1288,20 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="es-AR"/>
   <c:chart>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>'No Elementales'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -529,289 +1312,358 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>'No Elementales'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16384</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>350000</c:v>
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$12</c:f>
+              <c:f>'No Elementales'!$B$3:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$2</c:f>
+              <c:f>'No Elementales'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Quicksort</c:v>
+                  <c:v>QuickSort</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>'No Elementales'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16384</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>350000</c:v>
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$12</c:f>
+              <c:f>'No Elementales'!$C$3:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>61</c:v>
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$2</c:f>
+              <c:f>'No Elementales'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fusion</c:v>
+                  <c:v>Fusión</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>'No Elementales'!$A$3:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>20000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>30000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1000</c:v>
+                  <c:v>60000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1000</c:v>
+                  <c:v>70000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1000</c:v>
+                  <c:v>80000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16384</c:v>
+                  <c:v>90000</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>100000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>350000</c:v>
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>140000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>180000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$12</c:f>
+              <c:f>'No Elementales'!$D$3:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76</c:v>
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="71805184"/>
-        <c:axId val="71803648"/>
+        <c:axId val="49071616"/>
+        <c:axId val="49070080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71805184"/>
+        <c:axId val="49071616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71803648"/>
+        <c:crossAx val="49070080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71803648"/>
+        <c:axId val="49070080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +1671,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71805184"/>
+        <c:crossAx val="49071616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -895,6 +1747,76 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76197</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1188,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1201,66 +2123,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>0</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3">
         <v>0</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <v>0</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1268,25 +2190,25 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>10</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="3">
         <v>0</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <v>0</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1294,25 +2216,25 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1320,25 +2242,25 @@
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>10</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>0</v>
       </c>
     </row>
@@ -1346,25 +2268,25 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>1000</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>6</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <v>1</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>6</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
         <v>1</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <v>4</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>2</v>
       </c>
     </row>
@@ -1372,25 +2294,25 @@
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>1000</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>6</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <v>5</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>7</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <v>5</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1398,25 +2320,25 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>1000</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>6</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <v>5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>7</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
         <v>1</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1424,25 +2346,25 @@
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>16384</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>105</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <v>138</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>374</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
         <v>9</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="3">
         <v>10</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>15</v>
       </c>
     </row>
@@ -1450,25 +2372,25 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>100000</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>3694</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <v>4806</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>13963</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <v>16</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <v>29</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <v>37</v>
       </c>
     </row>
@@ -1476,43 +2398,27 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>350000</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>45214</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <v>59294</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>172975</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
         <v>41</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="3">
         <v>61</v>
       </c>
-      <c r="H12" s="5">
+      <c r="H12" s="3">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2097152</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5">
-        <v>245</v>
-      </c>
-      <c r="H13" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1528,24 +2434,493 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>894</v>
+      </c>
+      <c r="C3" s="3">
+        <v>362</v>
+      </c>
+      <c r="D3" s="3">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B4" s="3">
+        <v>2013</v>
+      </c>
+      <c r="C4" s="3">
+        <v>828</v>
+      </c>
+      <c r="D4" s="3">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>40000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3603</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1444</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5600</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2297</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
+        <v>60000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>8113</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3319</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>70000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10998</v>
+      </c>
+      <c r="C8" s="3">
+        <v>4432</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
+        <v>80000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>14363</v>
+      </c>
+      <c r="C9" s="3">
+        <v>5837</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5777</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
+        <v>90000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>18188</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7434</v>
+      </c>
+      <c r="D10" s="3">
+        <v>7308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>21280</v>
+      </c>
+      <c r="C11" s="3">
+        <v>9014</v>
+      </c>
+      <c r="D11" s="3">
+        <v>9032</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3">
+        <v>120000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>30692</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12996</v>
+      </c>
+      <c r="D12" s="3">
+        <v>12975</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>140000</v>
+      </c>
+      <c r="B13" s="3">
+        <v>43989</v>
+      </c>
+      <c r="C13" s="3">
+        <v>17638</v>
+      </c>
+      <c r="D13" s="3">
+        <v>17719</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3">
+        <v>160000</v>
+      </c>
+      <c r="B14" s="3">
+        <v>57558</v>
+      </c>
+      <c r="C14" s="3">
+        <v>23117</v>
+      </c>
+      <c r="D14" s="3">
+        <v>23094</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3">
+        <v>180000</v>
+      </c>
+      <c r="B15" s="3">
+        <v>73060</v>
+      </c>
+      <c r="C15" s="3">
+        <v>29386</v>
+      </c>
+      <c r="D15" s="3">
+        <v>29346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>200000</v>
+      </c>
+      <c r="B16" s="3">
+        <v>89752</v>
+      </c>
+      <c r="C16" s="3">
+        <v>36440</v>
+      </c>
+      <c r="D16" s="3">
+        <v>36163</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="E3:F16">
+    <sortCondition ref="E3:E16"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B4" s="3">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3">
+        <v>40000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5</v>
+      </c>
+      <c r="D5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="3">
+        <v>60000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="3">
+        <v>70000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>24</v>
+      </c>
+      <c r="C8" s="3">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="3">
+        <v>80000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="3">
+        <v>90000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>29</v>
+      </c>
+      <c r="C10" s="3">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="3">
+        <v>100000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>60</v>
+      </c>
+      <c r="C11" s="3">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="3">
+        <v>120000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3">
+        <v>18</v>
+      </c>
+      <c r="D12" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="3">
+        <v>140000</v>
+      </c>
+      <c r="B13" s="3">
+        <v>47</v>
+      </c>
+      <c r="C13" s="3">
+        <v>22</v>
+      </c>
+      <c r="D13" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="3">
+        <v>160000</v>
+      </c>
+      <c r="B14" s="3">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3">
+        <v>24</v>
+      </c>
+      <c r="D14" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="3">
+        <v>180000</v>
+      </c>
+      <c r="B15" s="3">
+        <v>69</v>
+      </c>
+      <c r="C15" s="3">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="3">
+        <v>200000</v>
+      </c>
+      <c r="B16" s="3">
+        <v>83</v>
+      </c>
+      <c r="C16" s="3">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A22:B34">
+    <sortCondition ref="A2:A15"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>